<commit_message>
add encode dummy function
</commit_message>
<xml_diff>
--- a/inst/features.xlsx
+++ b/inst/features.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
   <si>
     <t>Feature</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Allow the user to impute missing values</t>
   </si>
   <si>
-    <t>Encode nominal to numerical</t>
-  </si>
-  <si>
     <t>Allow the user to create "dummy" variables to represent nominal data</t>
   </si>
   <si>
@@ -225,6 +222,9 @@
   </si>
   <si>
     <t>button click</t>
+  </si>
+  <si>
+    <t>Create indicator variables</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,13 +649,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -681,19 +681,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>16</v>
@@ -713,19 +713,19 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>16</v>
@@ -745,7 +745,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>26</v>
@@ -777,19 +777,19 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>36</v>
@@ -809,19 +809,19 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>36</v>
@@ -841,19 +841,19 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>36</v>
@@ -864,26 +864,28 @@
     </row>
     <row r="9" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C9" s="2">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>36</v>
@@ -897,7 +899,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2">
         <v>9</v>
@@ -926,10 +928,10 @@
     </row>
     <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2">
         <v>10</v>
@@ -938,16 +940,16 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>36</v>
@@ -971,13 +973,13 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>36</v>

</xml_diff>